<commit_message>
updates on evaluation results
</commit_message>
<xml_diff>
--- a/data/manual_evaluation/results/counter_eval_sm.xlsx
+++ b/data/manual_evaluation/results/counter_eval_sm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sophi\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8180A10A-4263-4758-8393-9B428A335EFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C723CDA9-A2FA-462C-8A9D-3EF79EAA7C39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="105" windowWidth="16080" windowHeight="11340" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="eval_sample_all (1)" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="744">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1003" uniqueCount="746">
   <si>
     <t>ID</t>
   </si>
@@ -2262,6 +2262,12 @@
   </si>
   <si>
     <t>Opposes the argument, the language is argumentative and coherent, like all the other comments. This one is ranked four because is somewhat contradictory.</t>
+  </si>
+  <si>
+    <t>Addresses the argument on multiple points but, like all the other comments, does not opposes it. The language is argumentative and coherent</t>
+  </si>
+  <si>
+    <t>Addresses the argument but does not offer a single complete stance for or against,  instead, it gives you an argumentative cascade of possible responses, that lack coherency.</t>
   </si>
 </sst>
 </file>
@@ -2710,8 +2716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ401"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="B303" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B304" sqref="B304"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -6029,7 +6035,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="301" spans="1:5" ht="114.75">
+    <row r="301" spans="1:5" ht="127.5">
       <c r="C301" s="1" t="s">
         <v>454</v>
       </c>
@@ -6037,7 +6043,7 @@
         <v>1</v>
       </c>
       <c r="E301" s="1" t="s">
-        <v>695</v>
+        <v>744</v>
       </c>
     </row>
     <row r="302" spans="1:5" ht="242.25">
@@ -6050,18 +6056,27 @@
       <c r="C302" s="1" t="s">
         <v>457</v>
       </c>
+      <c r="D302" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="303" spans="1:5" ht="108.75" customHeight="1">
       <c r="C303" s="1" t="s">
         <v>458</v>
       </c>
       <c r="D303" s="1">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="E303" s="1" t="s">
+        <v>745</v>
       </c>
     </row>
     <row r="304" spans="1:5" ht="63.75">
       <c r="C304" s="1" t="s">
         <v>459</v>
+      </c>
+      <c r="D304" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="305" spans="1:5" ht="89.25">

</xml_diff>